<commit_message>
Mise à jour site peinture
</commit_message>
<xml_diff>
--- a/Prix/levis.xlsx
+++ b/Prix/levis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\levis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\peinture\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A3E8A1-E521-4751-A9C8-02088ADE7273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F773D0F6-5962-45F8-BF8E-F41DDDF48595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E95DC93-531D-460D-9A06-44397A8920D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="983">
   <si>
     <t>31100072</t>
   </si>
@@ -2934,6 +2934,57 @@
   </si>
   <si>
     <t>75,75lt 0001L</t>
+  </si>
+  <si>
+    <t>levis/Amb.lak-sat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Amb.lak.mat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Amb.mur-extra-mat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Amb.mur-metallic.jpg</t>
+  </si>
+  <si>
+    <t>levis/Amb.mur-satin.jpg</t>
+  </si>
+  <si>
+    <t>levis/Duo-sat-mix.jpg</t>
+  </si>
+  <si>
+    <t>levis/Easyclean-cuisine-sdb-mat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Easyclean-cuisine-sdb-sat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Easyclean-satin.jpg</t>
+  </si>
+  <si>
+    <t>levis/Expert-mur.jpg</t>
+  </si>
+  <si>
+    <t>levis/Facade-exp-levis-mix.png</t>
+  </si>
+  <si>
+    <t>levis/Ferro-decor.jpg</t>
+  </si>
+  <si>
+    <t>levis/Lak-exp-high-gloss.png</t>
+  </si>
+  <si>
+    <t>levis/Lak-exp-sat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Lak-rapide-exter.jpg</t>
+  </si>
+  <si>
+    <t>levis/Lak-reg-sat.jpg</t>
+  </si>
+  <si>
+    <t>levis/Levis-floor-regul.jpg</t>
   </si>
 </sst>
 </file>
@@ -3598,12 +3649,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065E4AF0-A4F8-4CE3-9E23-EDCEACB756BD}">
   <dimension ref="A1:G446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" style="3" customWidth="1"/>
@@ -3634,6 +3686,9 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>968</v>
+      </c>
       <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
@@ -3651,6 +3706,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>968</v>
+      </c>
       <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
@@ -3668,6 +3726,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>968</v>
+      </c>
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
@@ -3685,6 +3746,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>968</v>
+      </c>
       <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
@@ -3702,6 +3766,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>968</v>
+      </c>
       <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
@@ -3719,6 +3786,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>968</v>
+      </c>
       <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
@@ -3736,6 +3806,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>968</v>
+      </c>
       <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
@@ -3753,6 +3826,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>969</v>
+      </c>
       <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
@@ -3770,6 +3846,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>970</v>
+      </c>
       <c r="B10" s="13" t="s">
         <v>17</v>
       </c>
@@ -3787,6 +3866,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>970</v>
+      </c>
       <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
@@ -3804,6 +3886,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>970</v>
+      </c>
       <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
@@ -3821,6 +3906,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>970</v>
+      </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
@@ -3838,6 +3926,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>970</v>
+      </c>
       <c r="B14" s="14" t="s">
         <v>25</v>
       </c>
@@ -3855,6 +3946,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>970</v>
+      </c>
       <c r="B15" s="14" t="s">
         <v>27</v>
       </c>
@@ -3872,6 +3966,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>970</v>
+      </c>
       <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
@@ -3888,7 +3985,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>970</v>
+      </c>
       <c r="B17" s="15" t="s">
         <v>31</v>
       </c>
@@ -3905,7 +4005,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>970</v>
+      </c>
       <c r="B18" s="15" t="s">
         <v>33</v>
       </c>
@@ -3922,7 +4025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
@@ -3939,7 +4042,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>971</v>
+      </c>
       <c r="B20" s="16" t="s">
         <v>37</v>
       </c>
@@ -3956,7 +4062,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>971</v>
+      </c>
       <c r="B21" s="16" t="s">
         <v>39</v>
       </c>
@@ -3973,7 +4082,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>971</v>
+      </c>
       <c r="B22" s="16" t="s">
         <v>41</v>
       </c>
@@ -3990,7 +4102,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>971</v>
+      </c>
       <c r="B23" s="17" t="s">
         <v>43</v>
       </c>
@@ -4007,7 +4122,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>971</v>
+      </c>
       <c r="B24" s="17" t="s">
         <v>45</v>
       </c>
@@ -4024,7 +4142,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>971</v>
+      </c>
       <c r="B25" s="17" t="s">
         <v>47</v>
       </c>
@@ -4041,7 +4162,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>971</v>
+      </c>
       <c r="B26" s="18" t="s">
         <v>49</v>
       </c>
@@ -4058,7 +4182,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>971</v>
+      </c>
       <c r="B27" s="18" t="s">
         <v>51</v>
       </c>
@@ -4075,7 +4202,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>971</v>
+      </c>
       <c r="B28" s="18" t="s">
         <v>53</v>
       </c>
@@ -4092,7 +4222,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>967</v>
+      </c>
       <c r="B29" s="19" t="s">
         <v>55</v>
       </c>
@@ -4109,7 +4242,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>967</v>
+      </c>
       <c r="B30" s="19" t="s">
         <v>57</v>
       </c>
@@ -4126,7 +4262,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>967</v>
+      </c>
       <c r="B31" s="19" t="s">
         <v>59</v>
       </c>
@@ -4143,7 +4282,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>967</v>
+      </c>
       <c r="B32" s="20" t="s">
         <v>61</v>
       </c>
@@ -4160,7 +4302,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>967</v>
+      </c>
       <c r="B33" s="20" t="s">
         <v>63</v>
       </c>
@@ -4177,7 +4322,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>967</v>
+      </c>
       <c r="B34" s="20" t="s">
         <v>65</v>
       </c>
@@ -4194,7 +4342,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>967</v>
+      </c>
       <c r="B35" s="21" t="s">
         <v>67</v>
       </c>
@@ -4211,7 +4362,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>967</v>
+      </c>
       <c r="B36" s="21" t="s">
         <v>69</v>
       </c>
@@ -4228,7 +4382,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>967</v>
+      </c>
       <c r="B37" s="21" t="s">
         <v>71</v>
       </c>
@@ -4245,7 +4402,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>966</v>
+      </c>
       <c r="B38" s="22" t="s">
         <v>73</v>
       </c>
@@ -4262,7 +4422,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>966</v>
+      </c>
       <c r="B39" s="22" t="s">
         <v>75</v>
       </c>
@@ -4279,7 +4442,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>966</v>
+      </c>
       <c r="B40" s="22" t="s">
         <v>77</v>
       </c>
@@ -4296,7 +4462,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>966</v>
+      </c>
       <c r="B41" s="23" t="s">
         <v>79</v>
       </c>
@@ -4313,7 +4482,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>966</v>
+      </c>
       <c r="B42" s="23" t="s">
         <v>81</v>
       </c>
@@ -4330,7 +4502,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>966</v>
+      </c>
       <c r="B43" s="23" t="s">
         <v>83</v>
       </c>
@@ -4347,7 +4522,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>966</v>
+      </c>
       <c r="B44" s="24" t="s">
         <v>85</v>
       </c>
@@ -4364,7 +4542,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>966</v>
+      </c>
       <c r="B45" s="24" t="s">
         <v>87</v>
       </c>
@@ -4381,7 +4562,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>966</v>
+      </c>
       <c r="B46" s="24" t="s">
         <v>89</v>
       </c>
@@ -4398,7 +4582,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>975</v>
+      </c>
       <c r="B47" s="25" t="s">
         <v>91</v>
       </c>
@@ -4415,7 +4602,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>975</v>
+      </c>
       <c r="B48" s="25" t="s">
         <v>93</v>
       </c>
@@ -4432,7 +4622,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>975</v>
+      </c>
       <c r="B49" s="25" t="s">
         <v>95</v>
       </c>
@@ -4449,7 +4642,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>975</v>
+      </c>
       <c r="B50" s="26" t="s">
         <v>97</v>
       </c>
@@ -4466,7 +4662,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>975</v>
+      </c>
       <c r="B51" s="26" t="s">
         <v>99</v>
       </c>
@@ -4483,7 +4682,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>975</v>
+      </c>
       <c r="B52" s="26" t="s">
         <v>101</v>
       </c>
@@ -4500,7 +4702,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>975</v>
+      </c>
       <c r="B53" s="27" t="s">
         <v>103</v>
       </c>
@@ -4517,7 +4722,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>975</v>
+      </c>
       <c r="B54" s="27" t="s">
         <v>105</v>
       </c>
@@ -4534,7 +4742,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>975</v>
+      </c>
       <c r="B55" s="27" t="s">
         <v>107</v>
       </c>
@@ -4551,7 +4762,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>977</v>
+      </c>
       <c r="B56" s="28" t="s">
         <v>109</v>
       </c>
@@ -4568,7 +4782,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>977</v>
+      </c>
       <c r="B57" s="28" t="s">
         <v>111</v>
       </c>
@@ -4585,7 +4802,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>977</v>
+      </c>
       <c r="B58" s="28" t="s">
         <v>113</v>
       </c>
@@ -4602,7 +4822,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>977</v>
+      </c>
       <c r="B59" s="29" t="s">
         <v>115</v>
       </c>
@@ -4619,7 +4842,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>977</v>
+      </c>
       <c r="B60" s="29" t="s">
         <v>117</v>
       </c>
@@ -4636,7 +4862,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>977</v>
+      </c>
       <c r="B61" s="29" t="s">
         <v>119</v>
       </c>
@@ -4653,7 +4882,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>978</v>
+      </c>
       <c r="B62" s="30" t="s">
         <v>121</v>
       </c>
@@ -4670,7 +4902,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>978</v>
+      </c>
       <c r="B63" s="30" t="s">
         <v>123</v>
       </c>
@@ -4687,7 +4922,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>978</v>
+      </c>
       <c r="B64" s="30" t="s">
         <v>125</v>
       </c>
@@ -4704,7 +4942,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>978</v>
+      </c>
       <c r="B65" s="20" t="s">
         <v>127</v>
       </c>
@@ -4721,7 +4962,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>978</v>
+      </c>
       <c r="B66" s="20" t="s">
         <v>129</v>
       </c>
@@ -4738,7 +4982,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>978</v>
+      </c>
       <c r="B67" s="20" t="s">
         <v>131</v>
       </c>
@@ -4755,7 +5002,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>978</v>
+      </c>
       <c r="B68" s="21" t="s">
         <v>133</v>
       </c>
@@ -4772,7 +5022,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>978</v>
+      </c>
       <c r="B69" s="21" t="s">
         <v>135</v>
       </c>
@@ -4789,7 +5042,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>978</v>
+      </c>
       <c r="B70" s="21" t="s">
         <v>137</v>
       </c>
@@ -4806,7 +5062,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>979</v>
+      </c>
       <c r="B71" s="31" t="s">
         <v>139</v>
       </c>
@@ -4823,7 +5082,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>979</v>
+      </c>
       <c r="B72" s="31" t="s">
         <v>141</v>
       </c>
@@ -4840,7 +5102,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>979</v>
+      </c>
       <c r="B73" s="31" t="s">
         <v>143</v>
       </c>
@@ -4857,7 +5122,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>979</v>
+      </c>
       <c r="B74" s="32" t="s">
         <v>145</v>
       </c>
@@ -4874,7 +5142,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>979</v>
+      </c>
       <c r="B75" s="32" t="s">
         <v>147</v>
       </c>
@@ -4891,7 +5162,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>979</v>
+      </c>
       <c r="B76" s="32" t="s">
         <v>149</v>
       </c>
@@ -4908,7 +5182,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>979</v>
+      </c>
       <c r="B77" s="33" t="s">
         <v>151</v>
       </c>
@@ -4925,7 +5202,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>979</v>
+      </c>
       <c r="B78" s="33" t="s">
         <v>153</v>
       </c>
@@ -4942,7 +5222,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>979</v>
+      </c>
       <c r="B79" s="33" t="s">
         <v>155</v>
       </c>
@@ -4959,7 +5242,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>974</v>
+      </c>
       <c r="B80" s="16" t="s">
         <v>157</v>
       </c>
@@ -4976,7 +5262,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>974</v>
+      </c>
       <c r="B81" s="16" t="s">
         <v>159</v>
       </c>
@@ -4993,7 +5282,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>974</v>
+      </c>
       <c r="B82" s="17" t="s">
         <v>161</v>
       </c>
@@ -5010,7 +5302,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>974</v>
+      </c>
       <c r="B83" s="17" t="s">
         <v>163</v>
       </c>
@@ -5027,7 +5322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
@@ -5044,7 +5339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>165</v>
       </c>
@@ -5061,7 +5356,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>973</v>
+      </c>
       <c r="B86" s="27" t="s">
         <v>168</v>
       </c>
@@ -5078,7 +5376,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>973</v>
+      </c>
       <c r="B87" s="27" t="s">
         <v>170</v>
       </c>
@@ -5095,7 +5396,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>973</v>
+      </c>
       <c r="B88" s="28" t="s">
         <v>172</v>
       </c>
@@ -5112,7 +5416,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>973</v>
+      </c>
       <c r="B89" s="28" t="s">
         <v>174</v>
       </c>
@@ -5129,7 +5436,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>973</v>
+      </c>
       <c r="B90" s="29" t="s">
         <v>176</v>
       </c>
@@ -5146,7 +5456,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>973</v>
+      </c>
       <c r="B91" s="29" t="s">
         <v>178</v>
       </c>
@@ -5163,7 +5476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>180</v>
       </c>
@@ -5180,7 +5493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
         <v>182</v>
       </c>
@@ -5197,7 +5510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>184</v>
       </c>
@@ -5214,7 +5527,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>972</v>
+      </c>
       <c r="B95" s="22" t="s">
         <v>186</v>
       </c>
@@ -5231,7 +5547,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>972</v>
+      </c>
       <c r="B96" s="22" t="s">
         <v>188</v>
       </c>
@@ -5248,7 +5567,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>972</v>
+      </c>
       <c r="B97" s="23" t="s">
         <v>190</v>
       </c>
@@ -5265,7 +5587,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>972</v>
+      </c>
       <c r="B98" s="23" t="s">
         <v>192</v>
       </c>
@@ -5282,7 +5607,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>972</v>
+      </c>
       <c r="B99" s="24" t="s">
         <v>194</v>
       </c>
@@ -5299,7 +5627,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>972</v>
+      </c>
       <c r="B100" s="24" t="s">
         <v>196</v>
       </c>
@@ -5316,7 +5647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B101" s="2" t="s">
         <v>198</v>
       </c>
@@ -5333,7 +5664,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>980</v>
+      </c>
       <c r="B102" s="2" t="s">
         <v>200</v>
       </c>
@@ -5350,7 +5684,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>980</v>
+      </c>
       <c r="B103" s="31" t="s">
         <v>202</v>
       </c>
@@ -5367,7 +5704,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>980</v>
+      </c>
       <c r="B104" s="31" t="s">
         <v>204</v>
       </c>
@@ -5384,7 +5724,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>980</v>
+      </c>
       <c r="B105" s="32" t="s">
         <v>206</v>
       </c>
@@ -5401,7 +5744,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>980</v>
+      </c>
       <c r="B106" s="32" t="s">
         <v>208</v>
       </c>
@@ -5418,7 +5764,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>980</v>
+      </c>
       <c r="B107" s="32" t="s">
         <v>210</v>
       </c>
@@ -5435,7 +5784,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>980</v>
+      </c>
       <c r="B108" s="33" t="s">
         <v>212</v>
       </c>
@@ -5452,7 +5804,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>980</v>
+      </c>
       <c r="B109" s="33" t="s">
         <v>214</v>
       </c>
@@ -5469,7 +5824,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>980</v>
+      </c>
       <c r="B110" s="33" t="s">
         <v>216</v>
       </c>
@@ -5486,7 +5844,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>981</v>
+      </c>
       <c r="B111" s="34" t="s">
         <v>218</v>
       </c>
@@ -5503,7 +5864,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>981</v>
+      </c>
       <c r="B112" s="12" t="s">
         <v>220</v>
       </c>
@@ -5520,7 +5884,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>981</v>
+      </c>
       <c r="B113" s="12" t="s">
         <v>222</v>
       </c>
@@ -5537,7 +5904,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>981</v>
+      </c>
       <c r="B114" s="13" t="s">
         <v>224</v>
       </c>
@@ -5554,7 +5924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
         <v>226</v>
       </c>
@@ -5568,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
         <v>228</v>
       </c>
@@ -5585,7 +5955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
         <v>230</v>
       </c>
@@ -5602,7 +5972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="2" t="s">
         <v>232</v>
       </c>
@@ -5619,7 +5989,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>982</v>
+      </c>
       <c r="B119" s="22" t="s">
         <v>234</v>
       </c>
@@ -5636,7 +6009,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>982</v>
+      </c>
       <c r="B120" s="22" t="s">
         <v>236</v>
       </c>
@@ -5653,7 +6029,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>982</v>
+      </c>
       <c r="B121" s="23" t="s">
         <v>238</v>
       </c>
@@ -5670,7 +6049,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>976</v>
+      </c>
       <c r="B122" s="30" t="s">
         <v>240</v>
       </c>
@@ -5687,7 +6069,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>976</v>
+      </c>
       <c r="B123" s="30" t="s">
         <v>242</v>
       </c>
@@ -5704,7 +6089,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>976</v>
+      </c>
       <c r="B124" s="30" t="s">
         <v>244</v>
       </c>
@@ -5721,7 +6109,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>976</v>
+      </c>
       <c r="B125" s="35" t="s">
         <v>246</v>
       </c>
@@ -5738,7 +6129,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>976</v>
+      </c>
       <c r="B126" s="35" t="s">
         <v>248</v>
       </c>
@@ -5755,7 +6149,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>976</v>
+      </c>
       <c r="B127" s="35" t="s">
         <v>250</v>
       </c>
@@ -5772,7 +6169,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>976</v>
+      </c>
       <c r="B128" s="36" t="s">
         <v>252</v>
       </c>
@@ -5789,7 +6189,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>976</v>
+      </c>
       <c r="B129" s="36" t="s">
         <v>254</v>
       </c>
@@ -5806,7 +6209,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>976</v>
+      </c>
       <c r="B130" s="36" t="s">
         <v>256</v>
       </c>
@@ -5823,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B131" s="2" t="s">
         <v>258</v>
       </c>
@@ -5840,7 +6246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B132" s="2" t="s">
         <v>260</v>
       </c>
@@ -5857,7 +6263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B133" s="2" t="s">
         <v>262</v>
       </c>
@@ -5874,7 +6280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B134" s="2" t="s">
         <v>264</v>
       </c>
@@ -5891,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B135" s="2" t="s">
         <v>266</v>
       </c>
@@ -5908,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B136" s="2" t="s">
         <v>268</v>
       </c>
@@ -5925,7 +6331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B137" s="2" t="s">
         <v>270</v>
       </c>
@@ -5942,7 +6348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B138" s="2" t="s">
         <v>272</v>
       </c>
@@ -5959,7 +6365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B139" s="2" t="s">
         <v>581</v>
       </c>
@@ -5976,7 +6382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B140" s="2" t="s">
         <v>582</v>
       </c>
@@ -5993,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B141" s="2" t="s">
         <v>583</v>
       </c>
@@ -6010,7 +6416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B142" s="2" t="s">
         <v>584</v>
       </c>
@@ -6027,7 +6433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B143" s="2" t="s">
         <v>585</v>
       </c>
@@ -6044,7 +6450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B144" s="2" t="s">
         <v>586</v>
       </c>

</xml_diff>